<commit_message>
Positions value addition to events.
</commit_message>
<xml_diff>
--- a/templates/export/events.xlsx
+++ b/templates/export/events.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -933,7 +933,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +942,7 @@
     <col min="2" max="2" width="37.7109375" style="7" customWidth="1"/>
     <col min="3" max="3" width="37.28515625" style="7"/>
     <col min="4" max="4" width="38.5703125" style="7"/>
-    <col min="5" max="5" width="55.42578125" style="7"/>
+    <col min="5" max="5" width="72.28515625" style="7" customWidth="1"/>
     <col min="6" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Added course and permissive static filters
</commit_message>
<xml_diff>
--- a/templates/export/events.xlsx
+++ b/templates/export/events.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AAA69B-2B6D-3949-A1D1-1801AE12CE7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D94988-1755-C444-BD5C-CE49F6DF1912}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="1360" windowWidth="27820" windowHeight="17440" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5260" yWindow="7560" windowWidth="27820" windowHeight="17440" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -83,12 +83,6 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Geofence Name</t>
-  </si>
-  <si>
-    <t>Maintenance Name</t>
-  </si>
-  <si>
     <t>${event.type}</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>${maintenanceNames[event.maintenanceId]}</t>
   </si>
   <si>
-    <t>Activity Type</t>
-  </si>
-  <si>
     <t>Extended Values</t>
   </si>
   <si>
@@ -117,6 +108,15 @@
   </si>
   <si>
     <t>${event.attributes.toString().replaceAll(",", " ").replaceAll(bracketsRegex, "")}</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
   </si>
 </sst>
 </file>
@@ -918,7 +918,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -935,28 +935,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -968,19 +968,19 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>